<commit_message>
Agregando funcionalidad para soportar los conceptos OnAccount en la impresión del Invoice y el envio de notificacion por correo.
</commit_message>
<xml_diff>
--- a/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
+++ b/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AmigoDev\source\Amigo.Tenant.Application.Services.WebApi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60A1FC1-C6A6-42B4-9AEC-6574AACA72AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="336" windowWidth="15012" windowHeight="7692"/>
+    <workbookView xWindow="285" yWindow="330" windowWidth="15015" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$12:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$15:$G$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Invoice N°</t>
   </si>
@@ -64,12 +68,21 @@
   </si>
   <si>
     <t>V6B-1L8</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>PERIOD:</t>
+  </si>
+  <si>
+    <t>USER:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -223,7 +236,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -245,6 +258,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -257,12 +273,77 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39520</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109497</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5477003" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7ACE3-5C09-444A-8310-680D69927B06}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19165155">
+          <a:off x="39520" y="2947947"/>
+          <a:ext cx="5477003" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" cap="none" spc="50">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:alpha val="38000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:innerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>P A Y E D</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -278,7 +359,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -353,7 +440,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,9 +473,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,6 +525,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -596,26 +717,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40" style="1" customWidth="1"/>
-    <col min="4" max="6" width="12.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -623,460 +745,113 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="8" t="s">
+    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D26" s="9">
         <v>15000</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modificando Excel Paid por Payed
</commit_message>
<xml_diff>
--- a/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
+++ b/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AmigoDev\source\Amigo.Tenant.Application.Services.WebApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60A1FC1-C6A6-42B4-9AEC-6574AACA72AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F8AF90-4F89-4AC4-801D-FA6614ED2366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="330" windowWidth="15015" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,11 +255,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -337,7 +337,7 @@
                 </a:innerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>P A Y E D</a:t>
+            <a:t>P A I D</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -722,7 +722,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,12 +738,12 @@
   <sheetData>
     <row r="3" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -758,7 +758,7 @@
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -767,7 +767,7 @@
       <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">

</xml_diff>

<commit_message>
Correccion del Invoice para que genere el Balance
</commit_message>
<xml_diff>
--- a/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
+++ b/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AmigoDev\source\Amigo.Tenant.Application.Services.WebApi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F8AF90-4F89-4AC4-801D-FA6614ED2366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="330" windowWidth="15015" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="288" yWindow="336" windowWidth="15012" windowHeight="7692"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Invoice N°</t>
   </si>
@@ -77,16 +71,22 @@
   </si>
   <si>
     <t>USER:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance   </t>
+  </si>
+  <si>
+    <t>** If you have Late Fee this is not included as part of your debt in the balance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +179,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +206,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -230,13 +243,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -258,9 +286,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="1" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -295,10 +325,10 @@
         <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7ACE3-5C09-444A-8310-680D69927B06}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7ACE3-5C09-444A-8310-680D69927B06}"/>
             </a:ext>
             <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="0"/>
+              <adec:decorative xmlns="" xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="0"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -362,7 +392,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -440,7 +470,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -473,26 +503,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -525,23 +538,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,33 +713,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <pane ySplit="15" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="6" width="12.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -751,7 +747,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -760,7 +756,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -769,13 +765,13 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -784,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -793,29 +789,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
@@ -829,12 +825,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="3:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
@@ -842,13 +838,25 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Correccion de numeracion del Invoice
</commit_message>
<xml_diff>
--- a/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
+++ b/Amigo.Tenant.Application.Services.WebApi/AmigoInvoice.xlsx
@@ -264,7 +264,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -282,15 +282,24 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -325,10 +334,10 @@
         <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7ACE3-5C09-444A-8310-680D69927B06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71E7ACE3-5C09-444A-8310-680D69927B06}"/>
             </a:ext>
             <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns="" xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="0"/>
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -383,7 +392,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>112690</xdr:colOff>
+      <xdr:colOff>265090</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
@@ -392,7 +401,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -717,14 +726,14 @@
   <dimension ref="A3:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.5546875" style="1" customWidth="1"/>
@@ -734,12 +743,12 @@
   <sheetData>
     <row r="3" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -754,7 +763,7 @@
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -763,7 +772,7 @@
       <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -825,35 +834,68 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="9"/>
+    </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="13">
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="9"/>
+    </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="14"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1"/>

</xml_diff>